<commit_message>
starting to integrate error handling on Excel user inputs
</commit_message>
<xml_diff>
--- a/Building Blocks/Build_Foundation.xlsx
+++ b/Building Blocks/Build_Foundation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\REEDR-O\Building Blocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161885CD-DE38-4135-809A-89D6030B17AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AF2A85-B66B-4E65-A2DA-A526E379602B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D135BAC2-2A9D-498B-B692-4C5391A9D301}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D135BAC2-2A9D-498B-B692-4C5391A9D301}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -597,7 +597,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92667E3-9923-4324-8BDC-0F2F184C447E}">
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
@@ -608,20 +608,19 @@
     <col min="1" max="1" width="44.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="16.5703125" style="1" customWidth="1"/>
-    <col min="10" max="12" width="15.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="13" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="21.7109375" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="23.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="16.5703125" style="1" customWidth="1"/>
+    <col min="9" max="11" width="15.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -631,40 +630,39 @@
       <c r="C1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="G1" s="7" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -672,10 +670,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -683,15 +681,14 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
+      <c r="M2" s="4">
+        <v>0.5</v>
+      </c>
       <c r="N2" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="O2" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -699,19 +696,18 @@
         <v>2</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="M3" s="4">
+        <v>0.5</v>
+      </c>
       <c r="N3" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="O3" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -719,19 +715,18 @@
         <v>2</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="M4" s="4">
+        <v>0.5</v>
+      </c>
       <c r="N4" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="O4" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -739,19 +734,18 @@
         <v>2</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="M5" s="4">
+        <v>0.5</v>
+      </c>
       <c r="N5" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="O5" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -759,19 +753,18 @@
         <v>2</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="M6" s="4">
+        <v>0.5</v>
+      </c>
       <c r="N6" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="O6" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -781,16 +774,15 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="M7" s="4">
+        <v>0</v>
+      </c>
       <c r="N7" s="4">
         <v>0</v>
       </c>
-      <c r="O7" s="4">
-        <v>0</v>
-      </c>
-      <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O7" s="4"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -800,29 +792,28 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
       <c r="H8" s="4">
-        <v>0</v>
-      </c>
-      <c r="I8" s="4">
         <v>2</v>
       </c>
+      <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
+      <c r="M8" s="4">
+        <v>0</v>
+      </c>
       <c r="N8" s="4">
         <v>0</v>
       </c>
-      <c r="O8" s="4">
-        <v>0</v>
-      </c>
-      <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -832,29 +823,28 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
       <c r="H9" s="4">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
         <v>2</v>
       </c>
+      <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
       <c r="N9" s="4">
         <v>0</v>
       </c>
-      <c r="O9" s="4">
-        <v>0</v>
-      </c>
-      <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O9" s="4"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -864,33 +854,32 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
       <c r="H10" s="4">
-        <v>0</v>
-      </c>
-      <c r="I10" s="4">
         <v>2</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K10" s="4">
+      <c r="J10" s="4">
         <v>0.5</v>
       </c>
+      <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
+      <c r="M10" s="4">
+        <v>0</v>
+      </c>
       <c r="N10" s="4">
         <v>0</v>
       </c>
-      <c r="O10" s="4">
-        <v>0</v>
-      </c>
-      <c r="P10" s="4"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O10" s="4"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -900,33 +889,32 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
       <c r="H11" s="4">
-        <v>0</v>
-      </c>
-      <c r="I11" s="4">
         <v>2</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K11" s="4">
+      <c r="J11" s="4">
         <v>0.5</v>
       </c>
+      <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
       <c r="N11" s="4">
         <v>0</v>
       </c>
-      <c r="O11" s="4">
-        <v>0</v>
-      </c>
-      <c r="P11" s="4"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O11" s="4"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -936,27 +924,26 @@
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4" t="s">
+      <c r="I12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K12" s="4">
+      <c r="J12" s="4">
         <v>0.5</v>
       </c>
+      <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
       <c r="N12" s="4">
         <v>0</v>
       </c>
-      <c r="O12" s="4">
-        <v>0</v>
-      </c>
-      <c r="P12" s="4"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -966,27 +953,26 @@
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="4">
+      <c r="J13" s="4">
         <v>0.5</v>
       </c>
+      <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
       <c r="N13" s="4">
         <v>0</v>
       </c>
-      <c r="O13" s="4">
-        <v>0</v>
-      </c>
-      <c r="P13" s="4"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O13" s="4"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -996,8 +982,8 @@
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -1005,9 +991,8 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1017,7 +1002,7 @@
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -1027,9 +1012,8 @@
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1039,7 +1023,7 @@
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -1049,9 +1033,8 @@
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1061,7 +1044,7 @@
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -1071,9 +1054,8 @@
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1083,8 +1065,8 @@
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -1092,9 +1074,8 @@
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1104,7 +1085,7 @@
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
@@ -1114,9 +1095,8 @@
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1126,7 +1106,7 @@
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+      <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
@@ -1136,9 +1116,8 @@
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1148,7 +1127,7 @@
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -1158,9 +1137,8 @@
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1170,7 +1148,7 @@
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -1180,114 +1158,101 @@
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B22 D2:F22" xr:uid="{215A9823-175F-4791-911E-FBBBBEE8A6A6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B22 D2:E22" xr:uid="{215A9823-175F-4791-911E-FBBBBEE8A6A6}">
       <formula1>"Vented Crawlspace, Slab, Heated Basement, Unheated Basement"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>